<commit_message>
Slight form design modifications
</commit_message>
<xml_diff>
--- a/Testing Files/Determiner Test Files/CapstoneMLSDataTestingSmall.xlsx
+++ b/Testing Files/Determiner Test Files/CapstoneMLSDataTestingSmall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\HatcoMarketShareHelper\Testing FIles\Determiner Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837D9918-30AF-4FA9-94D9-0B5750D0839E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20714453-E390-4F61-BFA5-95C23BFC7882}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="706">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -2146,18 +2146,6 @@
   </si>
   <si>
     <t>1701 W 7th ST</t>
-  </si>
-  <si>
-    <t>Likely Closed</t>
-  </si>
-  <si>
-    <t>Escrow Officer</t>
-  </si>
-  <si>
-    <t>did not close</t>
-  </si>
-  <si>
-    <t>Marissa Graham</t>
   </si>
 </sst>
 </file>
@@ -3004,23 +2992,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O126"/>
+  <dimension ref="A1:M126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3060,14 +3048,8 @@
       <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>706</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>397</v>
       </c>
@@ -3104,11 +3086,8 @@
       <c r="L2" s="2">
         <v>228000</v>
       </c>
-      <c r="M2" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -3145,11 +3124,8 @@
       <c r="L3" s="2">
         <v>199000</v>
       </c>
-      <c r="M3" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3186,11 +3162,8 @@
       <c r="L4" s="2">
         <v>225990</v>
       </c>
-      <c r="M4" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3227,11 +3200,8 @@
       <c r="L5" s="2">
         <v>234990</v>
       </c>
-      <c r="M5" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -3265,11 +3235,8 @@
       <c r="L6" s="2">
         <v>175000</v>
       </c>
-      <c r="M6" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3306,11 +3273,8 @@
       <c r="L7" s="2">
         <v>168535</v>
       </c>
-      <c r="M7" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>222</v>
       </c>
@@ -3347,11 +3311,8 @@
       <c r="L8" s="2">
         <v>262000</v>
       </c>
-      <c r="M8" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>441</v>
       </c>
@@ -3388,11 +3349,8 @@
       <c r="L9" s="2">
         <v>235000</v>
       </c>
-      <c r="M9" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -3429,11 +3387,8 @@
       <c r="L10" s="2">
         <v>490000</v>
       </c>
-      <c r="M10" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>540</v>
       </c>
@@ -3467,11 +3422,8 @@
       <c r="L11" s="2">
         <v>129900</v>
       </c>
-      <c r="M11" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>391</v>
       </c>
@@ -3505,11 +3457,8 @@
       <c r="L12" s="2">
         <v>430000</v>
       </c>
-      <c r="M12" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3543,11 +3492,8 @@
       <c r="L13" s="2">
         <v>325000</v>
       </c>
-      <c r="M13" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>445</v>
       </c>
@@ -3584,11 +3530,8 @@
       <c r="L14" s="2">
         <v>177500</v>
       </c>
-      <c r="M14" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -3622,11 +3565,8 @@
       <c r="L15" s="2">
         <v>245160</v>
       </c>
-      <c r="M15" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>211</v>
       </c>
@@ -3663,11 +3603,8 @@
       <c r="L16" s="2">
         <v>280900</v>
       </c>
-      <c r="M16" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>488</v>
       </c>
@@ -3701,11 +3638,8 @@
       <c r="L17" s="2">
         <v>315000</v>
       </c>
-      <c r="M17" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>296</v>
       </c>
@@ -3739,11 +3673,8 @@
       <c r="L18" s="2">
         <v>235000</v>
       </c>
-      <c r="M18" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>267</v>
       </c>
@@ -3777,11 +3708,8 @@
       <c r="L19" s="2">
         <v>325000</v>
       </c>
-      <c r="M19" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>347</v>
       </c>
@@ -3818,11 +3746,8 @@
       <c r="L20" s="2">
         <v>503158</v>
       </c>
-      <c r="M20" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>408</v>
       </c>
@@ -3859,11 +3784,8 @@
       <c r="L21" s="2">
         <v>255000</v>
       </c>
-      <c r="M21" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>502</v>
       </c>
@@ -3900,11 +3822,8 @@
       <c r="L22" s="2">
         <v>185000</v>
       </c>
-      <c r="M22" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>275</v>
       </c>
@@ -3941,11 +3860,8 @@
       <c r="L23" s="2">
         <v>200000</v>
       </c>
-      <c r="M23" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>472</v>
       </c>
@@ -3982,11 +3898,8 @@
       <c r="L24" s="2">
         <v>255000</v>
       </c>
-      <c r="M24" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>313</v>
       </c>
@@ -4020,11 +3933,8 @@
       <c r="L25" s="2">
         <v>271990</v>
       </c>
-      <c r="M25" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>112</v>
       </c>
@@ -4061,14 +3971,8 @@
       <c r="L26" s="2">
         <v>345000</v>
       </c>
-      <c r="M26">
-        <v>20180931</v>
-      </c>
-      <c r="O26" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>268</v>
       </c>
@@ -4105,11 +4009,8 @@
       <c r="L27" s="2">
         <v>320000</v>
       </c>
-      <c r="M27" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -4143,11 +4044,8 @@
       <c r="L28" s="2">
         <v>58850</v>
       </c>
-      <c r="M28" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -4181,11 +4079,8 @@
       <c r="L29" s="2">
         <v>299900</v>
       </c>
-      <c r="M29" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -4219,11 +4114,8 @@
       <c r="L30" s="2">
         <v>102500</v>
       </c>
-      <c r="M30" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -4260,11 +4152,8 @@
       <c r="L31" s="2">
         <v>395000</v>
       </c>
-      <c r="M31" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -4298,11 +4187,8 @@
       <c r="L32" s="2">
         <v>299900</v>
       </c>
-      <c r="M32" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>494</v>
       </c>
@@ -4339,11 +4225,8 @@
       <c r="L33" s="2">
         <v>325000</v>
       </c>
-      <c r="M33" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -4380,11 +4263,8 @@
       <c r="L34" s="2">
         <v>230000</v>
       </c>
-      <c r="M34" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>171</v>
       </c>
@@ -4421,11 +4301,8 @@
       <c r="L35" s="2">
         <v>610000</v>
       </c>
-      <c r="M35" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -4462,11 +4339,8 @@
       <c r="L36" s="2">
         <v>269000</v>
       </c>
-      <c r="M36" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>124</v>
       </c>
@@ -4503,11 +4377,8 @@
       <c r="L37" s="2">
         <v>387500</v>
       </c>
-      <c r="M37" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -4544,11 +4415,8 @@
       <c r="L38" s="2">
         <v>375000</v>
       </c>
-      <c r="M38" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>587</v>
       </c>
@@ -4585,14 +4453,8 @@
       <c r="L39" s="2">
         <v>210000</v>
       </c>
-      <c r="M39">
-        <v>20180902</v>
-      </c>
-      <c r="O39" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -4626,11 +4488,8 @@
       <c r="L40" s="2">
         <v>555000</v>
       </c>
-      <c r="M40" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>511</v>
       </c>
@@ -4667,11 +4526,8 @@
       <c r="L41" s="2">
         <v>980000</v>
       </c>
-      <c r="M41" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>341</v>
       </c>
@@ -4708,11 +4564,8 @@
       <c r="L42" s="2">
         <v>419000</v>
       </c>
-      <c r="M42" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>551</v>
       </c>
@@ -4749,11 +4602,8 @@
       <c r="L43" s="2">
         <v>465000</v>
       </c>
-      <c r="M43" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>165</v>
       </c>
@@ -4790,11 +4640,8 @@
       <c r="L44" s="2">
         <v>230415</v>
       </c>
-      <c r="M44" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>686</v>
       </c>
@@ -4831,11 +4678,8 @@
       <c r="L45" s="2">
         <v>219325</v>
       </c>
-      <c r="M45" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>607</v>
       </c>
@@ -4872,11 +4716,8 @@
       <c r="L46" s="2">
         <v>325000</v>
       </c>
-      <c r="M46" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>516</v>
       </c>
@@ -4913,11 +4754,8 @@
       <c r="L47" s="2">
         <v>222000</v>
       </c>
-      <c r="M47" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>546</v>
       </c>
@@ -4954,11 +4792,8 @@
       <c r="L48" s="2">
         <v>254000</v>
       </c>
-      <c r="M48" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -4995,11 +4830,8 @@
       <c r="L49" s="2">
         <v>516900</v>
       </c>
-      <c r="M49" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -5033,11 +4865,8 @@
       <c r="L50" s="2">
         <v>135000</v>
       </c>
-      <c r="M50" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -5071,11 +4900,8 @@
       <c r="L51" s="2">
         <v>165900</v>
       </c>
-      <c r="M51" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -5109,11 +4935,8 @@
       <c r="L52" s="2">
         <v>288000</v>
       </c>
-      <c r="M52" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>394</v>
       </c>
@@ -5150,11 +4973,8 @@
       <c r="L53" s="2">
         <v>105000</v>
       </c>
-      <c r="M53" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>619</v>
       </c>
@@ -5191,11 +5011,8 @@
       <c r="L54" s="2">
         <v>182000</v>
       </c>
-      <c r="M54" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -5232,11 +5049,8 @@
       <c r="L55" s="2">
         <v>259000</v>
       </c>
-      <c r="M55" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>366</v>
       </c>
@@ -5273,11 +5087,8 @@
       <c r="L56" s="2">
         <v>350000</v>
       </c>
-      <c r="M56" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>437</v>
       </c>
@@ -5314,11 +5125,8 @@
       <c r="L57" s="2">
         <v>528000</v>
       </c>
-      <c r="M57" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>412</v>
       </c>
@@ -5355,11 +5163,8 @@
       <c r="L58" s="2">
         <v>309000</v>
       </c>
-      <c r="M58" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>402</v>
       </c>
@@ -5393,11 +5198,8 @@
       <c r="L59" s="2">
         <v>203000</v>
       </c>
-      <c r="M59" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>511</v>
       </c>
@@ -5434,11 +5236,8 @@
       <c r="L60" s="2">
         <v>215500</v>
       </c>
-      <c r="M60" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>480</v>
       </c>
@@ -5475,11 +5274,8 @@
       <c r="L61" s="2">
         <v>275000</v>
       </c>
-      <c r="M61" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>238</v>
       </c>
@@ -5516,11 +5312,8 @@
       <c r="L62" s="2">
         <v>320000</v>
       </c>
-      <c r="M62" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>531</v>
       </c>
@@ -5557,11 +5350,8 @@
       <c r="L63" s="2">
         <v>255900</v>
       </c>
-      <c r="M63" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>185</v>
       </c>
@@ -5598,11 +5388,8 @@
       <c r="L64" s="2">
         <v>325997</v>
       </c>
-      <c r="M64" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -5639,11 +5426,8 @@
       <c r="L65" s="2">
         <v>315000</v>
       </c>
-      <c r="M65" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>649</v>
       </c>
@@ -5680,11 +5464,8 @@
       <c r="L66" s="2">
         <v>249500</v>
       </c>
-      <c r="M66" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>214</v>
       </c>
@@ -5721,11 +5502,8 @@
       <c r="L67" s="2">
         <v>255000</v>
       </c>
-      <c r="M67" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>676</v>
       </c>
@@ -5762,11 +5540,8 @@
       <c r="L68" s="2">
         <v>407500</v>
       </c>
-      <c r="M68" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>24</v>
       </c>
@@ -5803,11 +5578,8 @@
       <c r="L69" s="2">
         <v>255900</v>
       </c>
-      <c r="M69" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>454</v>
       </c>
@@ -5844,11 +5616,8 @@
       <c r="L70" s="2">
         <v>230000</v>
       </c>
-      <c r="M70" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>681</v>
       </c>
@@ -5885,11 +5654,8 @@
       <c r="L71" s="2">
         <v>257500</v>
       </c>
-      <c r="M71" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>192</v>
       </c>
@@ -5926,11 +5692,8 @@
       <c r="L72" s="2">
         <v>535000</v>
       </c>
-      <c r="M72" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>45</v>
       </c>
@@ -5967,11 +5730,8 @@
       <c r="L73" s="2">
         <v>495000</v>
       </c>
-      <c r="M73" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -6008,11 +5768,8 @@
       <c r="L74" s="2">
         <v>235000</v>
       </c>
-      <c r="M74" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>533</v>
       </c>
@@ -6049,11 +5806,8 @@
       <c r="L75" s="2">
         <v>297500</v>
       </c>
-      <c r="M75" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>24</v>
       </c>
@@ -6090,11 +5844,8 @@
       <c r="L76" s="2">
         <v>184000</v>
       </c>
-      <c r="M76" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>553</v>
       </c>
@@ -6131,11 +5882,8 @@
       <c r="L77" s="2">
         <v>515000</v>
       </c>
-      <c r="M77" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>203</v>
       </c>
@@ -6169,11 +5917,8 @@
       <c r="L78" s="2">
         <v>270000</v>
       </c>
-      <c r="M78" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>239</v>
       </c>
@@ -6210,11 +5955,8 @@
       <c r="L79" s="2">
         <v>193300</v>
       </c>
-      <c r="M79" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>246</v>
       </c>
@@ -6248,11 +5990,8 @@
       <c r="L80" s="2">
         <v>211000</v>
       </c>
-      <c r="M80" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>172</v>
       </c>
@@ -6289,11 +6028,8 @@
       <c r="L81" s="2">
         <v>261500</v>
       </c>
-      <c r="M81" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>169</v>
       </c>
@@ -6330,11 +6066,8 @@
       <c r="L82" s="2">
         <v>294000</v>
       </c>
-      <c r="M82" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>216</v>
       </c>
@@ -6368,11 +6101,8 @@
       <c r="L83" s="2">
         <v>245000</v>
       </c>
-      <c r="M83" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>228</v>
       </c>
@@ -6409,11 +6139,8 @@
       <c r="L84" s="2">
         <v>293000</v>
       </c>
-      <c r="M84" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>150</v>
       </c>
@@ -6450,11 +6177,8 @@
       <c r="L85" s="2">
         <v>480500</v>
       </c>
-      <c r="M85" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>155</v>
       </c>
@@ -6491,11 +6215,8 @@
       <c r="L86" s="2">
         <v>550000</v>
       </c>
-      <c r="M86" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>227</v>
       </c>
@@ -6532,11 +6253,8 @@
       <c r="L87" s="2">
         <v>215000</v>
       </c>
-      <c r="M87" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>62</v>
       </c>
@@ -6573,11 +6291,8 @@
       <c r="L88" s="2">
         <v>300000</v>
       </c>
-      <c r="M88" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>598</v>
       </c>
@@ -6614,11 +6329,8 @@
       <c r="L89" s="2">
         <v>230000</v>
       </c>
-      <c r="M89" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>605</v>
       </c>
@@ -6655,11 +6367,8 @@
       <c r="L90" s="2">
         <v>266990</v>
       </c>
-      <c r="M90" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -6696,11 +6405,8 @@
       <c r="L91" s="2">
         <v>515000</v>
       </c>
-      <c r="M91" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>102</v>
       </c>
@@ -6737,11 +6443,8 @@
       <c r="L92" s="2">
         <v>287500</v>
       </c>
-      <c r="M92" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>57</v>
       </c>
@@ -6778,11 +6481,8 @@
       <c r="L93" s="2">
         <v>339000</v>
       </c>
-      <c r="M93" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -6816,11 +6516,8 @@
       <c r="L94" s="2">
         <v>201900</v>
       </c>
-      <c r="M94" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>381</v>
       </c>
@@ -6857,11 +6554,8 @@
       <c r="L95" s="2">
         <v>460000</v>
       </c>
-      <c r="M95" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>300</v>
       </c>
@@ -6898,11 +6592,8 @@
       <c r="L96" s="2">
         <v>255000</v>
       </c>
-      <c r="M96" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>354</v>
       </c>
@@ -6939,11 +6630,8 @@
       <c r="L97" s="2">
         <v>303000</v>
       </c>
-      <c r="M97" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>360</v>
       </c>
@@ -6980,11 +6668,8 @@
       <c r="L98" s="2">
         <v>350000</v>
       </c>
-      <c r="M98" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>236</v>
       </c>
@@ -7021,11 +6706,8 @@
       <c r="L99" s="2">
         <v>243500</v>
       </c>
-      <c r="M99" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>547</v>
       </c>
@@ -7062,11 +6744,8 @@
       <c r="L100" s="2">
         <v>320500</v>
       </c>
-      <c r="M100" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>24</v>
       </c>
@@ -7103,11 +6782,8 @@
       <c r="L101" s="2">
         <v>266050</v>
       </c>
-      <c r="M101" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>343</v>
       </c>
@@ -7141,11 +6817,8 @@
       <c r="L102" s="2">
         <v>258000</v>
       </c>
-      <c r="M102" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>423</v>
       </c>
@@ -7182,11 +6855,8 @@
       <c r="L103" s="2">
         <v>332000</v>
       </c>
-      <c r="M103" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>425</v>
       </c>
@@ -7223,11 +6893,8 @@
       <c r="L104" s="2">
         <v>361999</v>
       </c>
-      <c r="M104" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>404</v>
       </c>
@@ -7264,11 +6931,8 @@
       <c r="L105" s="2">
         <v>322500</v>
       </c>
-      <c r="M105" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>431</v>
       </c>
@@ -7305,11 +6969,8 @@
       <c r="L106" s="2">
         <v>391500</v>
       </c>
-      <c r="M106" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>111</v>
       </c>
@@ -7346,11 +7007,8 @@
       <c r="L107" s="2">
         <v>195000</v>
       </c>
-      <c r="M107" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>456</v>
       </c>
@@ -7387,11 +7045,8 @@
       <c r="L108" s="2">
         <v>201500</v>
       </c>
-      <c r="M108" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>478</v>
       </c>
@@ -7425,11 +7080,8 @@
       <c r="L109" s="2">
         <v>265000</v>
       </c>
-      <c r="M109" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>21</v>
       </c>
@@ -7466,11 +7118,8 @@
       <c r="L110" s="2">
         <v>217000</v>
       </c>
-      <c r="M110" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>304</v>
       </c>
@@ -7507,11 +7156,8 @@
       <c r="L111" s="2">
         <v>260000</v>
       </c>
-      <c r="M111" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>308</v>
       </c>
@@ -7548,11 +7194,8 @@
       <c r="L112" s="2">
         <v>265000</v>
       </c>
-      <c r="M112" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>328</v>
       </c>
@@ -7589,11 +7232,8 @@
       <c r="L113" s="2">
         <v>334350</v>
       </c>
-      <c r="M113" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>345</v>
       </c>
@@ -7627,11 +7267,8 @@
       <c r="L114" s="2">
         <v>485000</v>
       </c>
-      <c r="M114" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>421</v>
       </c>
@@ -7665,11 +7302,8 @@
       <c r="L115" s="2">
         <v>327232</v>
       </c>
-      <c r="M115" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>24</v>
       </c>
@@ -7706,11 +7340,8 @@
       <c r="L116" s="2">
         <v>304000</v>
       </c>
-      <c r="M116" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>560</v>
       </c>
@@ -7744,11 +7375,8 @@
       <c r="L117" s="2">
         <v>100000</v>
       </c>
-      <c r="M117" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>465</v>
       </c>
@@ -7785,11 +7413,8 @@
       <c r="L118" s="2">
         <v>190000</v>
       </c>
-      <c r="M118" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>119</v>
       </c>
@@ -7826,11 +7451,8 @@
       <c r="L119" s="2">
         <v>195000</v>
       </c>
-      <c r="M119" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>262</v>
       </c>
@@ -7867,11 +7489,8 @@
       <c r="L120" s="2">
         <v>191600</v>
       </c>
-      <c r="M120" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>640</v>
       </c>
@@ -7908,11 +7527,8 @@
       <c r="L121" s="2">
         <v>218000</v>
       </c>
-      <c r="M121" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>24</v>
       </c>
@@ -7949,11 +7565,8 @@
       <c r="L122" s="2">
         <v>229210</v>
       </c>
-      <c r="M122" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>450</v>
       </c>
@@ -7990,11 +7603,8 @@
       <c r="L123" s="2">
         <v>244900</v>
       </c>
-      <c r="M123" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>644</v>
       </c>
@@ -8031,11 +7641,8 @@
       <c r="L124" s="2">
         <v>256165</v>
       </c>
-      <c r="M124" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>658</v>
       </c>
@@ -8069,11 +7676,8 @@
       <c r="L125" s="2">
         <v>294000</v>
       </c>
-      <c r="M125" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>668</v>
       </c>
@@ -8110,12 +7714,9 @@
       <c r="L126" s="2">
         <v>355000</v>
       </c>
-      <c r="M126" t="s">
-        <v>708</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O126">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M126">
     <sortCondition ref="K2:K126"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>